<commit_message>
SNFI indicator 7 removed FSL indicator 2 removed WASH indicator 1 updated
</commit_message>
<xml_diff>
--- a/REACH_SOM_DSA4_combined_Indicators0804_DM_YS.xlsx
+++ b/REACH_SOM_DSA4_combined_Indicators0804_DM_YS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mac/Documents/REACH - Somalia/R/REACH_SOM_DSA_LSG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{833E1198-E601-A044-B29F-5D3DBAC92EE8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9812A94D-1E26-C148-92D5-AEB9DCF1FE46}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-6380" windowWidth="38400" windowHeight="21100" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1020" yWindow="500" windowWidth="27780" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="17" r:id="rId1"/>
@@ -178,7 +178,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5169" uniqueCount="2647">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5170" uniqueCount="2648">
   <si>
     <t>Code</t>
   </si>
@@ -8694,6 +8694,11 @@
   <si>
     <t>Children join/recruited by armed groups
 Displacement due to conflict</t>
+  </si>
+  <si>
+    <t>Do not treat water 
+&amp;
+River</t>
   </si>
 </sst>
 </file>
@@ -9760,6 +9765,12 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -9880,6 +9891,12 @@
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -9891,12 +9908,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -9930,12 +9941,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -18006,8 +18011,8 @@
   </sheetPr>
   <dimension ref="A1:R14"/>
   <sheetViews>
-    <sheetView zoomScale="108" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="108" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -18324,10 +18329,10 @@
       </c>
     </row>
     <row r="10" spans="1:18" s="61" customFormat="1" ht="136" x14ac:dyDescent="0.2">
-      <c r="A10" s="248" t="s">
+      <c r="A10" s="191" t="s">
         <v>2627</v>
       </c>
-      <c r="B10" s="248" t="s">
+      <c r="B10" s="191" t="s">
         <v>2638</v>
       </c>
       <c r="C10" s="15"/>
@@ -18436,8 +18441,8 @@
   </sheetPr>
   <dimension ref="A1:T18"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView topLeftCell="A3" zoomScale="97" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -18466,27 +18471,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="92" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="193" t="s">
+      <c r="B1" s="195" t="s">
         <v>892</v>
       </c>
-      <c r="C1" s="194"/>
-      <c r="D1" s="194"/>
-      <c r="E1" s="194"/>
-      <c r="F1" s="194"/>
-      <c r="G1" s="194"/>
-      <c r="H1" s="194"/>
-      <c r="I1" s="194"/>
-      <c r="J1" s="195"/>
-      <c r="K1" s="195"/>
-      <c r="L1" s="194"/>
-      <c r="M1" s="194"/>
-      <c r="N1" s="194"/>
-      <c r="O1" s="194"/>
-      <c r="P1" s="194"/>
-      <c r="Q1" s="194"/>
-      <c r="R1" s="194"/>
-      <c r="S1" s="194"/>
-      <c r="T1" s="196"/>
+      <c r="C1" s="196"/>
+      <c r="D1" s="196"/>
+      <c r="E1" s="196"/>
+      <c r="F1" s="196"/>
+      <c r="G1" s="196"/>
+      <c r="H1" s="196"/>
+      <c r="I1" s="196"/>
+      <c r="J1" s="197"/>
+      <c r="K1" s="197"/>
+      <c r="L1" s="196"/>
+      <c r="M1" s="196"/>
+      <c r="N1" s="196"/>
+      <c r="O1" s="196"/>
+      <c r="P1" s="196"/>
+      <c r="Q1" s="196"/>
+      <c r="R1" s="196"/>
+      <c r="S1" s="196"/>
+      <c r="T1" s="198"/>
     </row>
     <row r="2" spans="1:20" s="92" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="93"/>
@@ -18559,7 +18564,9 @@
       <c r="I3" s="77" t="s">
         <v>2548</v>
       </c>
-      <c r="J3" s="71"/>
+      <c r="J3" s="71" t="s">
+        <v>2647</v>
+      </c>
       <c r="K3" s="71"/>
       <c r="N3" s="58" t="s">
         <v>2601</v>
@@ -18669,27 +18676,27 @@
     </row>
     <row r="8" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:20" s="92" customFormat="1" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="197" t="s">
+      <c r="B9" s="199" t="s">
         <v>907</v>
       </c>
-      <c r="C9" s="198"/>
-      <c r="D9" s="198"/>
-      <c r="E9" s="198"/>
-      <c r="F9" s="199"/>
-      <c r="G9" s="199"/>
-      <c r="H9" s="199"/>
-      <c r="I9" s="199"/>
-      <c r="J9" s="199"/>
-      <c r="K9" s="199"/>
-      <c r="L9" s="198"/>
-      <c r="M9" s="198"/>
-      <c r="N9" s="198"/>
-      <c r="O9" s="198"/>
-      <c r="P9" s="198"/>
-      <c r="Q9" s="198"/>
-      <c r="R9" s="198"/>
-      <c r="S9" s="198"/>
-      <c r="T9" s="200"/>
+      <c r="C9" s="200"/>
+      <c r="D9" s="200"/>
+      <c r="E9" s="200"/>
+      <c r="F9" s="201"/>
+      <c r="G9" s="201"/>
+      <c r="H9" s="201"/>
+      <c r="I9" s="201"/>
+      <c r="J9" s="201"/>
+      <c r="K9" s="201"/>
+      <c r="L9" s="200"/>
+      <c r="M9" s="200"/>
+      <c r="N9" s="200"/>
+      <c r="O9" s="200"/>
+      <c r="P9" s="200"/>
+      <c r="Q9" s="200"/>
+      <c r="R9" s="200"/>
+      <c r="S9" s="200"/>
+      <c r="T9" s="202"/>
     </row>
     <row r="10" spans="1:20" s="92" customFormat="1" ht="13" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="53" t="s">
@@ -18704,16 +18711,16 @@
       <c r="E10" s="72" t="s">
         <v>895</v>
       </c>
-      <c r="F10" s="249"/>
-      <c r="G10" s="201" t="s">
+      <c r="F10" s="192"/>
+      <c r="G10" s="203" t="s">
         <v>908</v>
       </c>
-      <c r="H10" s="202"/>
-      <c r="I10" s="203" t="s">
+      <c r="H10" s="204"/>
+      <c r="I10" s="205" t="s">
         <v>909</v>
       </c>
-      <c r="J10" s="204"/>
-      <c r="K10" s="205"/>
+      <c r="J10" s="206"/>
+      <c r="K10" s="207"/>
       <c r="L10" s="72" t="s">
         <v>929</v>
       </c>
@@ -18754,15 +18761,15 @@
       <c r="E11" s="75" t="s">
         <v>950</v>
       </c>
-      <c r="G11" s="191" t="s">
+      <c r="G11" s="193" t="s">
         <v>951</v>
       </c>
-      <c r="H11" s="191"/>
-      <c r="I11" s="192" t="s">
+      <c r="H11" s="193"/>
+      <c r="I11" s="194" t="s">
         <v>952</v>
       </c>
-      <c r="J11" s="192"/>
-      <c r="K11" s="192"/>
+      <c r="J11" s="194"/>
+      <c r="K11" s="194"/>
       <c r="L11" s="109"/>
       <c r="M11" s="109"/>
       <c r="N11" s="110" t="s">
@@ -18791,15 +18798,15 @@
       <c r="E12" s="51" t="s">
         <v>954</v>
       </c>
-      <c r="G12" s="191" t="s">
+      <c r="G12" s="193" t="s">
         <v>955</v>
       </c>
-      <c r="H12" s="191"/>
-      <c r="I12" s="192" t="s">
+      <c r="H12" s="193"/>
+      <c r="I12" s="194" t="s">
         <v>956</v>
       </c>
-      <c r="J12" s="192"/>
-      <c r="K12" s="192"/>
+      <c r="J12" s="194"/>
+      <c r="K12" s="194"/>
       <c r="L12" s="113"/>
       <c r="M12" s="113"/>
       <c r="N12" s="58" t="s">
@@ -18825,15 +18832,15 @@
       <c r="E13" s="51" t="s">
         <v>957</v>
       </c>
-      <c r="G13" s="191" t="s">
+      <c r="G13" s="193" t="s">
         <v>958</v>
       </c>
-      <c r="H13" s="191"/>
-      <c r="I13" s="192" t="s">
+      <c r="H13" s="193"/>
+      <c r="I13" s="194" t="s">
         <v>959</v>
       </c>
-      <c r="J13" s="192"/>
-      <c r="K13" s="192"/>
+      <c r="J13" s="194"/>
+      <c r="K13" s="194"/>
       <c r="L13" s="113"/>
       <c r="M13" s="113"/>
       <c r="N13" s="58" t="s">
@@ -18859,15 +18866,15 @@
       <c r="E14" s="51" t="s">
         <v>960</v>
       </c>
-      <c r="G14" s="191" t="s">
+      <c r="G14" s="193" t="s">
         <v>961</v>
       </c>
-      <c r="H14" s="191"/>
-      <c r="I14" s="192" t="s">
+      <c r="H14" s="193"/>
+      <c r="I14" s="194" t="s">
         <v>962</v>
       </c>
-      <c r="J14" s="192"/>
-      <c r="K14" s="192"/>
+      <c r="J14" s="194"/>
+      <c r="K14" s="194"/>
       <c r="L14" s="113"/>
       <c r="M14" s="113"/>
       <c r="N14" s="58" t="s">
@@ -18890,15 +18897,15 @@
       <c r="E15" s="51" t="s">
         <v>2564</v>
       </c>
-      <c r="G15" s="191" t="s">
+      <c r="G15" s="193" t="s">
         <v>958</v>
       </c>
-      <c r="H15" s="191"/>
-      <c r="I15" s="192" t="s">
+      <c r="H15" s="193"/>
+      <c r="I15" s="194" t="s">
         <v>959</v>
       </c>
-      <c r="J15" s="192"/>
-      <c r="K15" s="192"/>
+      <c r="J15" s="194"/>
+      <c r="K15" s="194"/>
       <c r="L15" s="113"/>
       <c r="M15" s="113"/>
       <c r="N15" s="16" t="s">
@@ -18943,13 +18950,13 @@
         <v>2621</v>
       </c>
       <c r="H17" s="76"/>
-      <c r="I17" s="192" t="s">
+      <c r="I17" s="194" t="s">
         <v>2563</v>
       </c>
-      <c r="J17" s="192" t="s">
+      <c r="J17" s="194" t="s">
         <v>946</v>
       </c>
-      <c r="K17" s="192"/>
+      <c r="K17" s="194"/>
       <c r="N17" s="58" t="s">
         <v>2562</v>
       </c>
@@ -18997,8 +19004,8 @@
   </sheetPr>
   <dimension ref="A1:V17"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9:J17"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -19022,28 +19029,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" s="52" customFormat="1" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C1" s="207" t="s">
+      <c r="C1" s="209" t="s">
         <v>892</v>
       </c>
-      <c r="D1" s="207"/>
-      <c r="E1" s="207"/>
-      <c r="F1" s="207"/>
-      <c r="G1" s="207"/>
-      <c r="H1" s="207"/>
-      <c r="I1" s="207"/>
-      <c r="J1" s="207"/>
-      <c r="K1" s="207"/>
-      <c r="L1" s="207"/>
-      <c r="M1" s="207"/>
-      <c r="N1" s="207"/>
-      <c r="O1" s="207"/>
-      <c r="P1" s="207"/>
-      <c r="Q1" s="207"/>
-      <c r="R1" s="207"/>
-      <c r="S1" s="207"/>
-      <c r="T1" s="207"/>
-      <c r="U1" s="207"/>
-      <c r="V1" s="207"/>
+      <c r="D1" s="209"/>
+      <c r="E1" s="209"/>
+      <c r="F1" s="209"/>
+      <c r="G1" s="209"/>
+      <c r="H1" s="209"/>
+      <c r="I1" s="209"/>
+      <c r="J1" s="209"/>
+      <c r="K1" s="209"/>
+      <c r="L1" s="209"/>
+      <c r="M1" s="209"/>
+      <c r="N1" s="209"/>
+      <c r="O1" s="209"/>
+      <c r="P1" s="209"/>
+      <c r="Q1" s="209"/>
+      <c r="R1" s="209"/>
+      <c r="S1" s="209"/>
+      <c r="T1" s="209"/>
+      <c r="U1" s="209"/>
+      <c r="V1" s="209"/>
     </row>
     <row r="2" spans="1:22" s="116" customFormat="1" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C2" s="37" t="s">
@@ -19238,28 +19245,28 @@
       <c r="V6" s="73"/>
     </row>
     <row r="7" spans="1:22" s="92" customFormat="1" ht="13.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="197" t="s">
+      <c r="C7" s="199" t="s">
         <v>907</v>
       </c>
-      <c r="D7" s="198"/>
-      <c r="E7" s="198"/>
-      <c r="F7" s="198"/>
-      <c r="G7" s="198"/>
-      <c r="H7" s="198"/>
-      <c r="I7" s="199"/>
-      <c r="J7" s="199"/>
-      <c r="K7" s="199"/>
-      <c r="L7" s="199"/>
-      <c r="M7" s="199"/>
-      <c r="N7" s="198"/>
-      <c r="O7" s="198"/>
-      <c r="P7" s="198"/>
-      <c r="Q7" s="198"/>
-      <c r="R7" s="198"/>
-      <c r="S7" s="198"/>
-      <c r="T7" s="198"/>
-      <c r="U7" s="198"/>
-      <c r="V7" s="200"/>
+      <c r="D7" s="200"/>
+      <c r="E7" s="200"/>
+      <c r="F7" s="200"/>
+      <c r="G7" s="200"/>
+      <c r="H7" s="200"/>
+      <c r="I7" s="201"/>
+      <c r="J7" s="201"/>
+      <c r="K7" s="201"/>
+      <c r="L7" s="201"/>
+      <c r="M7" s="201"/>
+      <c r="N7" s="200"/>
+      <c r="O7" s="200"/>
+      <c r="P7" s="200"/>
+      <c r="Q7" s="200"/>
+      <c r="R7" s="200"/>
+      <c r="S7" s="200"/>
+      <c r="T7" s="200"/>
+      <c r="U7" s="200"/>
+      <c r="V7" s="202"/>
     </row>
     <row r="8" spans="1:22" s="92" customFormat="1" ht="13.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C8" s="53" t="s">
@@ -19278,15 +19285,15 @@
       <c r="H8" s="72" t="s">
         <v>895</v>
       </c>
-      <c r="I8" s="208" t="s">
+      <c r="I8" s="210" t="s">
         <v>908</v>
       </c>
-      <c r="J8" s="209"/>
-      <c r="K8" s="210" t="s">
+      <c r="J8" s="211"/>
+      <c r="K8" s="212" t="s">
         <v>909</v>
       </c>
-      <c r="L8" s="211"/>
-      <c r="M8" s="212"/>
+      <c r="L8" s="213"/>
+      <c r="M8" s="214"/>
       <c r="N8" s="72" t="s">
         <v>929</v>
       </c>
@@ -19325,10 +19332,10 @@
       <c r="H9" s="54" t="s">
         <v>2530</v>
       </c>
-      <c r="I9" s="206" t="s">
+      <c r="I9" s="208" t="s">
         <v>2566</v>
       </c>
-      <c r="J9" s="206"/>
+      <c r="J9" s="208"/>
       <c r="K9" s="77" t="s">
         <v>1809</v>
       </c>
@@ -19357,10 +19364,10 @@
       <c r="H10" s="54" t="s">
         <v>2531</v>
       </c>
-      <c r="I10" s="206" t="s">
+      <c r="I10" s="208" t="s">
         <v>2567</v>
       </c>
-      <c r="J10" s="206"/>
+      <c r="J10" s="208"/>
       <c r="K10" s="77" t="s">
         <v>1638</v>
       </c>
@@ -19388,10 +19395,10 @@
       <c r="H11" s="54" t="s">
         <v>2535</v>
       </c>
-      <c r="I11" s="206" t="s">
+      <c r="I11" s="208" t="s">
         <v>2551</v>
       </c>
-      <c r="J11" s="206"/>
+      <c r="J11" s="208"/>
       <c r="K11" s="77" t="s">
         <v>2550</v>
       </c>
@@ -19419,10 +19426,10 @@
       <c r="H12" s="55" t="s">
         <v>2537</v>
       </c>
-      <c r="I12" s="206" t="s">
+      <c r="I12" s="208" t="s">
         <v>2551</v>
       </c>
-      <c r="J12" s="206"/>
+      <c r="J12" s="208"/>
       <c r="K12" s="77" t="s">
         <v>2550</v>
       </c>
@@ -19450,10 +19457,10 @@
       <c r="H13" s="55" t="s">
         <v>2538</v>
       </c>
-      <c r="I13" s="206" t="s">
+      <c r="I13" s="208" t="s">
         <v>2551</v>
       </c>
-      <c r="J13" s="206"/>
+      <c r="J13" s="208"/>
       <c r="K13" s="77" t="s">
         <v>2550</v>
       </c>
@@ -19481,10 +19488,10 @@
       <c r="H14" s="55" t="s">
         <v>2539</v>
       </c>
-      <c r="I14" s="206" t="s">
+      <c r="I14" s="208" t="s">
         <v>2551</v>
       </c>
-      <c r="J14" s="206"/>
+      <c r="J14" s="208"/>
       <c r="K14" s="77" t="s">
         <v>2550</v>
       </c>
@@ -19512,10 +19519,10 @@
       <c r="H15" s="55" t="s">
         <v>2540</v>
       </c>
-      <c r="I15" s="206" t="s">
+      <c r="I15" s="208" t="s">
         <v>2551</v>
       </c>
-      <c r="J15" s="206"/>
+      <c r="J15" s="208"/>
       <c r="K15" s="77" t="s">
         <v>2550</v>
       </c>
@@ -19543,10 +19550,10 @@
       <c r="H16" s="55" t="s">
         <v>2547</v>
       </c>
-      <c r="I16" s="206" t="s">
+      <c r="I16" s="208" t="s">
         <v>2551</v>
       </c>
-      <c r="J16" s="206"/>
+      <c r="J16" s="208"/>
       <c r="K16" s="77" t="s">
         <v>2550</v>
       </c>
@@ -19572,10 +19579,10 @@
       <c r="H17" s="54" t="s">
         <v>2541</v>
       </c>
-      <c r="I17" s="206" t="s">
+      <c r="I17" s="208" t="s">
         <v>982</v>
       </c>
-      <c r="J17" s="206"/>
+      <c r="J17" s="208"/>
       <c r="K17" s="77" t="s">
         <v>2534</v>
       </c>
@@ -19642,26 +19649,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" s="62" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C1" s="213" t="s">
+      <c r="C1" s="215" t="s">
         <v>892</v>
       </c>
-      <c r="D1" s="213"/>
-      <c r="E1" s="213"/>
-      <c r="F1" s="213"/>
-      <c r="G1" s="213"/>
-      <c r="H1" s="213"/>
-      <c r="I1" s="213"/>
-      <c r="J1" s="213"/>
-      <c r="K1" s="213"/>
-      <c r="L1" s="213"/>
-      <c r="M1" s="213"/>
-      <c r="N1" s="213"/>
-      <c r="O1" s="213"/>
-      <c r="P1" s="213"/>
-      <c r="Q1" s="213"/>
-      <c r="R1" s="213"/>
-      <c r="S1" s="213"/>
-      <c r="T1" s="213"/>
+      <c r="D1" s="215"/>
+      <c r="E1" s="215"/>
+      <c r="F1" s="215"/>
+      <c r="G1" s="215"/>
+      <c r="H1" s="215"/>
+      <c r="I1" s="215"/>
+      <c r="J1" s="215"/>
+      <c r="K1" s="215"/>
+      <c r="L1" s="215"/>
+      <c r="M1" s="215"/>
+      <c r="N1" s="215"/>
+      <c r="O1" s="215"/>
+      <c r="P1" s="215"/>
+      <c r="Q1" s="215"/>
+      <c r="R1" s="215"/>
+      <c r="S1" s="215"/>
+      <c r="T1" s="215"/>
     </row>
     <row r="2" spans="1:23" s="62" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C2" s="37" t="s">
@@ -19770,26 +19777,26 @@
     </row>
     <row r="5" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="6" spans="1:23" s="36" customFormat="1" ht="11" x14ac:dyDescent="0.15">
-      <c r="C6" s="214" t="s">
+      <c r="C6" s="216" t="s">
         <v>907</v>
       </c>
-      <c r="D6" s="215"/>
-      <c r="E6" s="215"/>
-      <c r="F6" s="215"/>
-      <c r="G6" s="215"/>
-      <c r="H6" s="215"/>
-      <c r="I6" s="215"/>
-      <c r="J6" s="215"/>
-      <c r="K6" s="215"/>
-      <c r="L6" s="215"/>
-      <c r="M6" s="215"/>
-      <c r="N6" s="215"/>
-      <c r="O6" s="215"/>
-      <c r="P6" s="215"/>
-      <c r="Q6" s="215"/>
-      <c r="R6" s="215"/>
-      <c r="S6" s="215"/>
-      <c r="T6" s="216"/>
+      <c r="D6" s="217"/>
+      <c r="E6" s="217"/>
+      <c r="F6" s="217"/>
+      <c r="G6" s="217"/>
+      <c r="H6" s="217"/>
+      <c r="I6" s="217"/>
+      <c r="J6" s="217"/>
+      <c r="K6" s="217"/>
+      <c r="L6" s="217"/>
+      <c r="M6" s="217"/>
+      <c r="N6" s="217"/>
+      <c r="O6" s="217"/>
+      <c r="P6" s="217"/>
+      <c r="Q6" s="217"/>
+      <c r="R6" s="217"/>
+      <c r="S6" s="217"/>
+      <c r="T6" s="218"/>
     </row>
     <row r="7" spans="1:23" s="36" customFormat="1" ht="12" x14ac:dyDescent="0.15">
       <c r="C7" s="37" t="s">
@@ -19804,15 +19811,15 @@
       <c r="F7" s="40" t="s">
         <v>895</v>
       </c>
-      <c r="G7" s="217" t="s">
+      <c r="G7" s="219" t="s">
         <v>908</v>
       </c>
-      <c r="H7" s="217"/>
-      <c r="I7" s="218" t="s">
+      <c r="H7" s="219"/>
+      <c r="I7" s="220" t="s">
         <v>909</v>
       </c>
-      <c r="J7" s="218"/>
-      <c r="K7" s="219"/>
+      <c r="J7" s="220"/>
+      <c r="K7" s="221"/>
       <c r="L7" s="37" t="s">
         <v>929</v>
       </c>
@@ -19932,7 +19939,7 @@
   </sheetPr>
   <dimension ref="A1:T17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -19957,26 +19964,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="146" customFormat="1" ht="12" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="C1" s="220" t="s">
+      <c r="C1" s="222" t="s">
         <v>892</v>
       </c>
-      <c r="D1" s="220"/>
-      <c r="E1" s="220"/>
-      <c r="F1" s="220"/>
-      <c r="G1" s="220"/>
-      <c r="H1" s="220"/>
-      <c r="I1" s="220"/>
-      <c r="J1" s="220"/>
-      <c r="K1" s="220"/>
-      <c r="L1" s="220"/>
-      <c r="M1" s="220"/>
-      <c r="N1" s="220"/>
-      <c r="O1" s="220"/>
-      <c r="P1" s="220"/>
-      <c r="Q1" s="220"/>
-      <c r="R1" s="220"/>
-      <c r="S1" s="220"/>
-      <c r="T1" s="220"/>
+      <c r="D1" s="222"/>
+      <c r="E1" s="222"/>
+      <c r="F1" s="222"/>
+      <c r="G1" s="222"/>
+      <c r="H1" s="222"/>
+      <c r="I1" s="222"/>
+      <c r="J1" s="222"/>
+      <c r="K1" s="222"/>
+      <c r="L1" s="222"/>
+      <c r="M1" s="222"/>
+      <c r="N1" s="222"/>
+      <c r="O1" s="222"/>
+      <c r="P1" s="222"/>
+      <c r="Q1" s="222"/>
+      <c r="R1" s="222"/>
+      <c r="S1" s="222"/>
+      <c r="T1" s="222"/>
     </row>
     <row r="2" spans="1:20" s="146" customFormat="1" ht="37" thickBot="1" x14ac:dyDescent="0.2">
       <c r="C2" s="40" t="s">
@@ -20125,26 +20132,26 @@
       <c r="O5" s="151"/>
     </row>
     <row r="6" spans="1:20" s="146" customFormat="1" ht="12" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="C6" s="221" t="s">
+      <c r="C6" s="223" t="s">
         <v>907</v>
       </c>
-      <c r="D6" s="222"/>
-      <c r="E6" s="222"/>
-      <c r="F6" s="222"/>
-      <c r="G6" s="222"/>
-      <c r="H6" s="222"/>
-      <c r="I6" s="222"/>
-      <c r="J6" s="222"/>
-      <c r="K6" s="222"/>
-      <c r="L6" s="222"/>
-      <c r="M6" s="222"/>
-      <c r="N6" s="222"/>
-      <c r="O6" s="222"/>
-      <c r="P6" s="222"/>
-      <c r="Q6" s="222"/>
-      <c r="R6" s="222"/>
-      <c r="S6" s="222"/>
-      <c r="T6" s="223"/>
+      <c r="D6" s="224"/>
+      <c r="E6" s="224"/>
+      <c r="F6" s="224"/>
+      <c r="G6" s="224"/>
+      <c r="H6" s="224"/>
+      <c r="I6" s="224"/>
+      <c r="J6" s="224"/>
+      <c r="K6" s="224"/>
+      <c r="L6" s="224"/>
+      <c r="M6" s="224"/>
+      <c r="N6" s="224"/>
+      <c r="O6" s="224"/>
+      <c r="P6" s="224"/>
+      <c r="Q6" s="224"/>
+      <c r="R6" s="224"/>
+      <c r="S6" s="224"/>
+      <c r="T6" s="225"/>
     </row>
     <row r="7" spans="1:20" s="146" customFormat="1" ht="37" thickBot="1" x14ac:dyDescent="0.2">
       <c r="C7" s="40" t="s">
@@ -20159,15 +20166,15 @@
       <c r="F7" s="40" t="s">
         <v>895</v>
       </c>
-      <c r="G7" s="224" t="s">
+      <c r="G7" s="226" t="s">
         <v>908</v>
       </c>
-      <c r="H7" s="224"/>
-      <c r="I7" s="225" t="s">
+      <c r="H7" s="226"/>
+      <c r="I7" s="227" t="s">
         <v>909</v>
       </c>
-      <c r="J7" s="225"/>
-      <c r="K7" s="226"/>
+      <c r="J7" s="227"/>
+      <c r="K7" s="228"/>
       <c r="L7" s="40" t="s">
         <v>929</v>
       </c>
@@ -20206,15 +20213,15 @@
       <c r="F8" s="60" t="s">
         <v>989</v>
       </c>
-      <c r="G8" s="229" t="s">
+      <c r="G8" s="231" t="s">
         <v>912</v>
       </c>
-      <c r="H8" s="229"/>
-      <c r="I8" s="230" t="s">
+      <c r="H8" s="231"/>
+      <c r="I8" s="232" t="s">
         <v>913</v>
       </c>
-      <c r="J8" s="230"/>
-      <c r="K8" s="230"/>
+      <c r="J8" s="232"/>
+      <c r="K8" s="232"/>
       <c r="N8" s="152" t="s">
         <v>721</v>
       </c>
@@ -20238,15 +20245,15 @@
       <c r="F9" s="55" t="s">
         <v>991</v>
       </c>
-      <c r="G9" s="191" t="s">
+      <c r="G9" s="193" t="s">
         <v>2584</v>
       </c>
-      <c r="H9" s="191"/>
-      <c r="I9" s="192" t="s">
+      <c r="H9" s="193"/>
+      <c r="I9" s="194" t="s">
         <v>992</v>
       </c>
-      <c r="J9" s="192"/>
-      <c r="K9" s="192"/>
+      <c r="J9" s="194"/>
+      <c r="K9" s="194"/>
       <c r="N9" s="154" t="s">
         <v>663</v>
       </c>
@@ -20270,15 +20277,15 @@
       <c r="D10" s="14"/>
       <c r="E10" s="14"/>
       <c r="F10" s="16"/>
-      <c r="G10" s="191" t="s">
+      <c r="G10" s="193" t="s">
         <v>2586</v>
       </c>
-      <c r="H10" s="191"/>
-      <c r="I10" s="192" t="s">
+      <c r="H10" s="193"/>
+      <c r="I10" s="194" t="s">
         <v>2587</v>
       </c>
-      <c r="J10" s="192"/>
-      <c r="K10" s="192"/>
+      <c r="J10" s="194"/>
+      <c r="K10" s="194"/>
       <c r="N10" s="58" t="s">
         <v>2585</v>
       </c>
@@ -20290,11 +20297,11 @@
       </c>
     </row>
     <row r="11" spans="1:20" s="146" customFormat="1" ht="11" x14ac:dyDescent="0.15">
-      <c r="G11" s="227"/>
-      <c r="H11" s="227"/>
-      <c r="I11" s="228"/>
-      <c r="J11" s="228"/>
-      <c r="K11" s="228"/>
+      <c r="G11" s="229"/>
+      <c r="H11" s="229"/>
+      <c r="I11" s="230"/>
+      <c r="J11" s="230"/>
+      <c r="K11" s="230"/>
     </row>
     <row r="14" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D14" s="14"/>
@@ -20360,7 +20367,7 @@
   </sheetPr>
   <dimension ref="A1:T21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
@@ -20380,26 +20387,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="52" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C1" s="231" t="s">
+      <c r="C1" s="235" t="s">
         <v>907</v>
       </c>
-      <c r="D1" s="232"/>
-      <c r="E1" s="232"/>
-      <c r="F1" s="232"/>
-      <c r="G1" s="233"/>
-      <c r="H1" s="233"/>
-      <c r="I1" s="233"/>
-      <c r="J1" s="233"/>
-      <c r="K1" s="233"/>
-      <c r="L1" s="232"/>
-      <c r="M1" s="232"/>
-      <c r="N1" s="232"/>
-      <c r="O1" s="232"/>
-      <c r="P1" s="232"/>
-      <c r="Q1" s="232"/>
-      <c r="R1" s="232"/>
-      <c r="S1" s="232"/>
-      <c r="T1" s="234"/>
+      <c r="D1" s="236"/>
+      <c r="E1" s="236"/>
+      <c r="F1" s="236"/>
+      <c r="G1" s="237"/>
+      <c r="H1" s="237"/>
+      <c r="I1" s="237"/>
+      <c r="J1" s="237"/>
+      <c r="K1" s="237"/>
+      <c r="L1" s="236"/>
+      <c r="M1" s="236"/>
+      <c r="N1" s="236"/>
+      <c r="O1" s="236"/>
+      <c r="P1" s="236"/>
+      <c r="Q1" s="236"/>
+      <c r="R1" s="236"/>
+      <c r="S1" s="236"/>
+      <c r="T1" s="238"/>
     </row>
     <row r="2" spans="1:20" s="52" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C2" s="44" t="s">
@@ -20414,15 +20421,15 @@
       <c r="F2" s="44" t="s">
         <v>895</v>
       </c>
-      <c r="G2" s="237" t="s">
+      <c r="G2" s="239" t="s">
         <v>908</v>
       </c>
-      <c r="H2" s="238"/>
-      <c r="I2" s="239" t="s">
+      <c r="H2" s="240"/>
+      <c r="I2" s="241" t="s">
         <v>909</v>
       </c>
-      <c r="J2" s="239"/>
-      <c r="K2" s="240"/>
+      <c r="J2" s="241"/>
+      <c r="K2" s="242"/>
       <c r="L2" s="43" t="s">
         <v>929</v>
       </c>
@@ -20461,15 +20468,15 @@
       <c r="F3" s="54" t="s">
         <v>995</v>
       </c>
-      <c r="G3" s="235" t="s">
+      <c r="G3" s="233" t="s">
         <v>996</v>
       </c>
-      <c r="H3" s="235"/>
-      <c r="I3" s="236" t="s">
+      <c r="H3" s="233"/>
+      <c r="I3" s="234" t="s">
         <v>997</v>
       </c>
-      <c r="J3" s="236"/>
-      <c r="K3" s="236"/>
+      <c r="J3" s="234"/>
+      <c r="K3" s="234"/>
       <c r="N3" s="87" t="s">
         <v>604</v>
       </c>
@@ -20496,15 +20503,15 @@
       <c r="F4" s="54" t="s">
         <v>2615</v>
       </c>
-      <c r="G4" s="235" t="s">
+      <c r="G4" s="233" t="s">
         <v>2572</v>
       </c>
-      <c r="H4" s="235"/>
-      <c r="I4" s="236">
+      <c r="H4" s="233"/>
+      <c r="I4" s="234">
         <v>0</v>
       </c>
-      <c r="J4" s="236"/>
-      <c r="K4" s="236"/>
+      <c r="J4" s="234"/>
+      <c r="K4" s="234"/>
       <c r="N4" s="117" t="s">
         <v>1000</v>
       </c>
@@ -20528,15 +20535,15 @@
       <c r="F5" s="54" t="s">
         <v>1001</v>
       </c>
-      <c r="G5" s="235" t="s">
+      <c r="G5" s="233" t="s">
         <v>952</v>
       </c>
-      <c r="H5" s="235"/>
-      <c r="I5" s="236" t="s">
+      <c r="H5" s="233"/>
+      <c r="I5" s="234" t="s">
         <v>951</v>
       </c>
-      <c r="J5" s="236"/>
-      <c r="K5" s="236"/>
+      <c r="J5" s="234"/>
+      <c r="K5" s="234"/>
       <c r="N5" s="87" t="s">
         <v>638</v>
       </c>
@@ -20560,15 +20567,15 @@
       <c r="F6" s="54" t="s">
         <v>1002</v>
       </c>
-      <c r="G6" s="235" t="s">
+      <c r="G6" s="233" t="s">
         <v>952</v>
       </c>
-      <c r="H6" s="235"/>
-      <c r="I6" s="236" t="s">
+      <c r="H6" s="233"/>
+      <c r="I6" s="234" t="s">
         <v>951</v>
       </c>
-      <c r="J6" s="236"/>
-      <c r="K6" s="236"/>
+      <c r="J6" s="234"/>
+      <c r="K6" s="234"/>
       <c r="N6" s="87" t="s">
         <v>641</v>
       </c>
@@ -20592,15 +20599,15 @@
       <c r="F7" s="54" t="s">
         <v>1003</v>
       </c>
-      <c r="G7" s="235" t="s">
+      <c r="G7" s="233" t="s">
         <v>966</v>
       </c>
-      <c r="H7" s="235"/>
-      <c r="I7" s="236" t="s">
+      <c r="H7" s="233"/>
+      <c r="I7" s="234" t="s">
         <v>1004</v>
       </c>
-      <c r="J7" s="236"/>
-      <c r="K7" s="236"/>
+      <c r="J7" s="234"/>
+      <c r="K7" s="234"/>
       <c r="N7" s="87" t="s">
         <v>644</v>
       </c>
@@ -20624,15 +20631,15 @@
       <c r="F8" s="54" t="s">
         <v>2589</v>
       </c>
-      <c r="G8" s="191" t="s">
+      <c r="G8" s="193" t="s">
         <v>2593</v>
       </c>
-      <c r="H8" s="191"/>
-      <c r="I8" s="192" t="s">
+      <c r="H8" s="193"/>
+      <c r="I8" s="194" t="s">
         <v>2594</v>
       </c>
-      <c r="J8" s="192"/>
-      <c r="K8" s="192"/>
+      <c r="J8" s="194"/>
+      <c r="K8" s="194"/>
       <c r="N8" s="16" t="s">
         <v>609</v>
       </c>
@@ -20647,15 +20654,15 @@
       <c r="F9" s="54" t="s">
         <v>2590</v>
       </c>
-      <c r="G9" s="191" t="s">
+      <c r="G9" s="193" t="s">
         <v>2595</v>
       </c>
-      <c r="H9" s="191"/>
-      <c r="I9" s="192" t="s">
+      <c r="H9" s="193"/>
+      <c r="I9" s="194" t="s">
         <v>2596</v>
       </c>
-      <c r="J9" s="192"/>
-      <c r="K9" s="192"/>
+      <c r="J9" s="194"/>
+      <c r="K9" s="194"/>
       <c r="N9" s="16" t="s">
         <v>609</v>
       </c>
@@ -20670,15 +20677,15 @@
       <c r="F10" s="54" t="s">
         <v>2592</v>
       </c>
-      <c r="G10" s="191" t="s">
+      <c r="G10" s="193" t="s">
         <v>2597</v>
       </c>
-      <c r="H10" s="191"/>
-      <c r="I10" s="192" t="s">
+      <c r="H10" s="193"/>
+      <c r="I10" s="194" t="s">
         <v>2598</v>
       </c>
-      <c r="J10" s="192"/>
-      <c r="K10" s="192"/>
+      <c r="J10" s="194"/>
+      <c r="K10" s="194"/>
       <c r="N10" s="16" t="s">
         <v>609</v>
       </c>
@@ -20693,15 +20700,15 @@
       <c r="F11" s="54" t="s">
         <v>2591</v>
       </c>
-      <c r="G11" s="191" t="s">
+      <c r="G11" s="193" t="s">
         <v>2599</v>
       </c>
-      <c r="H11" s="191"/>
-      <c r="I11" s="192" t="s">
+      <c r="H11" s="193"/>
+      <c r="I11" s="194" t="s">
         <v>2600</v>
       </c>
-      <c r="J11" s="192"/>
-      <c r="K11" s="192"/>
+      <c r="J11" s="194"/>
+      <c r="K11" s="194"/>
       <c r="N11" s="16" t="s">
         <v>609</v>
       </c>
@@ -20716,26 +20723,26 @@
       <c r="N14" s="16"/>
     </row>
     <row r="15" spans="1:20" s="52" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="231" t="s">
+      <c r="C15" s="235" t="s">
         <v>2618</v>
       </c>
-      <c r="D15" s="232"/>
-      <c r="E15" s="232"/>
-      <c r="F15" s="232"/>
-      <c r="G15" s="233"/>
-      <c r="H15" s="233"/>
-      <c r="I15" s="233"/>
-      <c r="J15" s="233"/>
-      <c r="K15" s="233"/>
-      <c r="L15" s="232"/>
-      <c r="M15" s="232"/>
-      <c r="N15" s="232"/>
-      <c r="O15" s="232"/>
-      <c r="P15" s="232"/>
-      <c r="Q15" s="232"/>
-      <c r="R15" s="232"/>
-      <c r="S15" s="232"/>
-      <c r="T15" s="234"/>
+      <c r="D15" s="236"/>
+      <c r="E15" s="236"/>
+      <c r="F15" s="236"/>
+      <c r="G15" s="237"/>
+      <c r="H15" s="237"/>
+      <c r="I15" s="237"/>
+      <c r="J15" s="237"/>
+      <c r="K15" s="237"/>
+      <c r="L15" s="236"/>
+      <c r="M15" s="236"/>
+      <c r="N15" s="236"/>
+      <c r="O15" s="236"/>
+      <c r="P15" s="236"/>
+      <c r="Q15" s="236"/>
+      <c r="R15" s="236"/>
+      <c r="S15" s="236"/>
+      <c r="T15" s="238"/>
     </row>
     <row r="16" spans="1:20" s="146" customFormat="1" ht="25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="C16" s="40" t="s">
@@ -20878,13 +20885,6 @@
     <row r="21" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="I4:K4"/>
-    <mergeCell ref="C1:T1"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:K3"/>
     <mergeCell ref="C15:T15"/>
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="I5:K5"/>
@@ -20900,6 +20900,13 @@
     <mergeCell ref="I10:K10"/>
     <mergeCell ref="G11:H11"/>
     <mergeCell ref="I11:K11"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:K4"/>
+    <mergeCell ref="C1:T1"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:K3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -20936,26 +20943,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:19" s="52" customFormat="1" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="207" t="s">
+      <c r="B1" s="209" t="s">
         <v>892</v>
       </c>
-      <c r="C1" s="207"/>
-      <c r="D1" s="207"/>
-      <c r="E1" s="207"/>
-      <c r="F1" s="207"/>
-      <c r="G1" s="207"/>
-      <c r="H1" s="207"/>
-      <c r="I1" s="207"/>
-      <c r="J1" s="207"/>
-      <c r="K1" s="207"/>
-      <c r="L1" s="207"/>
-      <c r="M1" s="207"/>
-      <c r="N1" s="207"/>
-      <c r="O1" s="207"/>
-      <c r="P1" s="207"/>
-      <c r="Q1" s="207"/>
-      <c r="R1" s="207"/>
-      <c r="S1" s="207"/>
+      <c r="C1" s="209"/>
+      <c r="D1" s="209"/>
+      <c r="E1" s="209"/>
+      <c r="F1" s="209"/>
+      <c r="G1" s="209"/>
+      <c r="H1" s="209"/>
+      <c r="I1" s="209"/>
+      <c r="J1" s="209"/>
+      <c r="K1" s="209"/>
+      <c r="L1" s="209"/>
+      <c r="M1" s="209"/>
+      <c r="N1" s="209"/>
+      <c r="O1" s="209"/>
+      <c r="P1" s="209"/>
+      <c r="Q1" s="209"/>
+      <c r="R1" s="209"/>
+      <c r="S1" s="209"/>
     </row>
     <row r="2" spans="2:19" s="52" customFormat="1" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="44" t="s">
@@ -21080,26 +21087,26 @@
       </c>
     </row>
     <row r="5" spans="2:19" s="62" customFormat="1" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="214" t="s">
+      <c r="B5" s="216" t="s">
         <v>907</v>
       </c>
-      <c r="C5" s="215"/>
-      <c r="D5" s="215"/>
-      <c r="E5" s="215"/>
-      <c r="F5" s="243"/>
-      <c r="G5" s="243"/>
-      <c r="H5" s="243"/>
-      <c r="I5" s="243"/>
-      <c r="J5" s="243"/>
-      <c r="K5" s="215"/>
-      <c r="L5" s="215"/>
-      <c r="M5" s="215"/>
-      <c r="N5" s="215"/>
-      <c r="O5" s="215"/>
-      <c r="P5" s="215"/>
-      <c r="Q5" s="215"/>
-      <c r="R5" s="215"/>
-      <c r="S5" s="216"/>
+      <c r="C5" s="217"/>
+      <c r="D5" s="217"/>
+      <c r="E5" s="217"/>
+      <c r="F5" s="245"/>
+      <c r="G5" s="245"/>
+      <c r="H5" s="245"/>
+      <c r="I5" s="245"/>
+      <c r="J5" s="245"/>
+      <c r="K5" s="217"/>
+      <c r="L5" s="217"/>
+      <c r="M5" s="217"/>
+      <c r="N5" s="217"/>
+      <c r="O5" s="217"/>
+      <c r="P5" s="217"/>
+      <c r="Q5" s="217"/>
+      <c r="R5" s="217"/>
+      <c r="S5" s="218"/>
     </row>
     <row r="6" spans="2:19" s="62" customFormat="1" ht="12" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B6" s="37" t="s">
@@ -21114,15 +21121,15 @@
       <c r="E6" s="37" t="s">
         <v>895</v>
       </c>
-      <c r="F6" s="244" t="s">
+      <c r="F6" s="246" t="s">
         <v>908</v>
       </c>
-      <c r="G6" s="245"/>
-      <c r="H6" s="246" t="s">
+      <c r="G6" s="247"/>
+      <c r="H6" s="248" t="s">
         <v>909</v>
       </c>
-      <c r="I6" s="246"/>
-      <c r="J6" s="247"/>
+      <c r="I6" s="248"/>
+      <c r="J6" s="249"/>
       <c r="K6" s="38" t="s">
         <v>929</v>
       </c>
@@ -21158,15 +21165,15 @@
       <c r="E7" s="61" t="s">
         <v>1014</v>
       </c>
-      <c r="F7" s="241" t="s">
+      <c r="F7" s="243" t="s">
         <v>912</v>
       </c>
-      <c r="G7" s="241"/>
-      <c r="H7" s="242" t="s">
+      <c r="G7" s="243"/>
+      <c r="H7" s="244" t="s">
         <v>913</v>
       </c>
-      <c r="I7" s="242"/>
-      <c r="J7" s="242"/>
+      <c r="I7" s="244"/>
+      <c r="J7" s="244"/>
       <c r="M7" s="80" t="s">
         <v>734</v>
       </c>
@@ -21184,15 +21191,15 @@
       <c r="E8" s="61" t="s">
         <v>1015</v>
       </c>
-      <c r="F8" s="241" t="s">
+      <c r="F8" s="243" t="s">
         <v>912</v>
       </c>
-      <c r="G8" s="241"/>
-      <c r="H8" s="242" t="s">
+      <c r="G8" s="243"/>
+      <c r="H8" s="244" t="s">
         <v>913</v>
       </c>
-      <c r="I8" s="242"/>
-      <c r="J8" s="242"/>
+      <c r="I8" s="244"/>
+      <c r="J8" s="244"/>
       <c r="M8" s="80" t="s">
         <v>737</v>
       </c>
@@ -21210,15 +21217,15 @@
       <c r="E9" s="61" t="s">
         <v>1016</v>
       </c>
-      <c r="F9" s="241" t="s">
+      <c r="F9" s="243" t="s">
         <v>913</v>
       </c>
-      <c r="G9" s="241"/>
-      <c r="H9" s="242" t="s">
+      <c r="G9" s="243"/>
+      <c r="H9" s="244" t="s">
         <v>912</v>
       </c>
-      <c r="I9" s="242"/>
-      <c r="J9" s="242"/>
+      <c r="I9" s="244"/>
+      <c r="J9" s="244"/>
       <c r="M9" s="80" t="s">
         <v>754</v>
       </c>
@@ -21236,15 +21243,15 @@
       <c r="E10" s="61" t="s">
         <v>1017</v>
       </c>
-      <c r="F10" s="241" t="s">
+      <c r="F10" s="243" t="s">
         <v>913</v>
       </c>
-      <c r="G10" s="241"/>
-      <c r="H10" s="242" t="s">
+      <c r="G10" s="243"/>
+      <c r="H10" s="244" t="s">
         <v>912</v>
       </c>
-      <c r="I10" s="242"/>
-      <c r="J10" s="242"/>
+      <c r="I10" s="244"/>
+      <c r="J10" s="244"/>
       <c r="M10" s="80" t="s">
         <v>757</v>
       </c>

</xml_diff>